<commit_message>
Modif Hebdo 5, ajout hebdo 6
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine5.xlsx
+++ b/meeting/GestionHedbo_Semaine5.xlsx
@@ -213,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,6 +232,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -406,7 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,17 +444,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -457,12 +466,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -846,10 +853,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -858,12 +865,12 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -884,15 +891,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -902,45 +909,45 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="35"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -954,15 +961,15 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,7 +1027,7 @@
       <c r="C13" s="9">
         <v>41336</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="36"/>
       <c r="F13" s="11">
         <v>1</v>
@@ -1036,7 +1043,7 @@
       <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="36"/>
       <c r="F14" s="11">
         <v>3</v>
@@ -1068,7 +1075,7 @@
       <c r="C16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="36"/>
       <c r="F16" s="14">
         <v>6</v>
@@ -1096,7 +1103,7 @@
       <c r="C18" s="9">
         <v>41336</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="36">
         <v>162</v>
       </c>
@@ -1117,7 +1124,7 @@
       <c r="C19" s="9">
         <v>41336</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="36"/>
       <c r="F19" s="11">
         <v>1</v>
@@ -1133,7 +1140,7 @@
       <c r="C20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="36"/>
       <c r="F20" s="11">
         <v>3</v>
@@ -1149,7 +1156,7 @@
       <c r="C21" s="9">
         <v>41336</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="36"/>
       <c r="F21" s="11">
         <v>1</v>
@@ -1165,7 +1172,7 @@
       <c r="C22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="31"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="36"/>
       <c r="F22" s="11">
         <v>5</v>
@@ -1179,7 +1186,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="36"/>
-      <c r="F23" s="17"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="36"/>
       <c r="H23" s="5"/>
     </row>
@@ -1193,7 +1200,7 @@
       <c r="C24" s="9">
         <v>41336</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="36">
         <v>152</v>
       </c>
@@ -1214,7 +1221,7 @@
       <c r="C25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="36"/>
       <c r="F25" s="11">
         <v>2</v>
@@ -1230,7 +1237,7 @@
       <c r="C26" s="9">
         <v>41336</v>
       </c>
-      <c r="D26" s="12"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="36"/>
       <c r="F26" s="11">
         <v>3</v>
@@ -1246,7 +1253,7 @@
       <c r="C27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="36"/>
       <c r="F27" s="11">
         <v>4</v>
@@ -1259,10 +1266,10 @@
       <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="27"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="36"/>
       <c r="F28" s="15">
         <v>1</v>
@@ -1280,7 +1287,7 @@
       <c r="C29" s="9">
         <v>41336</v>
       </c>
-      <c r="D29" s="16"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="36">
         <v>145</v>
       </c>
@@ -1301,7 +1308,7 @@
       <c r="C30" s="9">
         <v>41336</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="27" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="36"/>
@@ -1319,7 +1326,7 @@
       <c r="C31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="26"/>
       <c r="E31" s="36"/>
       <c r="F31" s="11">
         <v>2</v>
@@ -1335,7 +1342,7 @@
       <c r="C32" s="9">
         <v>41336</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="36"/>
       <c r="F32" s="11">
         <v>3</v>
@@ -1345,15 +1352,15 @@
     </row>
     <row r="33" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="38"/>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="36"/>
-      <c r="F33" s="21">
+      <c r="F33" s="20">
         <v>1</v>
       </c>
       <c r="G33" s="36"/>
@@ -1367,7 +1374,7 @@
       <c r="C34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="36"/>
       <c r="F34" s="15">
         <v>6</v>
@@ -1385,7 +1392,7 @@
       <c r="C35" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="28"/>
       <c r="E35" s="37">
         <v>156</v>
       </c>
@@ -1406,7 +1413,7 @@
       <c r="C36" s="9">
         <v>41336</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="37"/>
       <c r="F36" s="11">
         <v>3</v>
@@ -1422,7 +1429,7 @@
       <c r="C37" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="37"/>
       <c r="F37" s="11">
         <v>2</v>
@@ -1438,7 +1445,7 @@
       <c r="C38" s="9">
         <v>41336</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="37"/>
       <c r="F38" s="11">
         <v>1</v>
@@ -1454,7 +1461,7 @@
       <c r="C39" s="9">
         <v>41336</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="37"/>
       <c r="F39" s="11">
         <v>3</v>
@@ -1469,10 +1476,10 @@
       <c r="B40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="23"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="37">
         <v>141</v>
       </c>
@@ -1493,7 +1500,7 @@
       <c r="C41" s="9">
         <v>41336</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="37"/>
       <c r="F41" s="11">
         <v>3</v>
@@ -1509,7 +1516,7 @@
       <c r="C42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="12"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="37"/>
       <c r="F42" s="11">
         <v>2</v>
@@ -1525,7 +1532,7 @@
       <c r="C43" s="9">
         <v>41336</v>
       </c>
-      <c r="D43" s="12"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="37"/>
       <c r="F43" s="11">
         <v>1</v>
@@ -1541,7 +1548,7 @@
       <c r="C44" s="9">
         <v>41336</v>
       </c>
-      <c r="D44" s="12"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="37"/>
       <c r="F44" s="11">
         <v>3</v>
@@ -1557,7 +1564,7 @@
       <c r="C45" s="9">
         <v>41336</v>
       </c>
-      <c r="D45" s="12"/>
+      <c r="D45" s="26"/>
       <c r="E45" s="37"/>
       <c r="F45" s="11">
         <v>4</v>
@@ -1573,7 +1580,7 @@
       <c r="C46" s="9">
         <v>41336</v>
       </c>
-      <c r="D46" s="12"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="37"/>
       <c r="F46" s="11">
         <v>3</v>
@@ -1591,7 +1598,7 @@
       <c r="C47" s="9">
         <v>41336</v>
       </c>
-      <c r="D47" s="12"/>
+      <c r="D47" s="26"/>
       <c r="E47" s="36">
         <v>140</v>
       </c>
@@ -1612,7 +1619,7 @@
       <c r="C48" s="9">
         <v>41336</v>
       </c>
-      <c r="D48" s="12"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="36"/>
       <c r="F48" s="11">
         <v>1</v>
@@ -1625,10 +1632,10 @@
       <c r="B49" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="27"/>
+      <c r="D49" s="26"/>
       <c r="E49" s="36"/>
       <c r="F49" s="11">
         <v>2</v>
@@ -1641,10 +1648,10 @@
       <c r="B50" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="30"/>
+      <c r="D50" s="29"/>
       <c r="E50" s="36"/>
       <c r="F50" s="11">
         <v>4</v>
@@ -1660,7 +1667,7 @@
       <c r="C51" s="9">
         <v>41336</v>
       </c>
-      <c r="D51" s="12"/>
+      <c r="D51" s="27"/>
       <c r="E51" s="36"/>
       <c r="F51" s="11">
         <v>4</v>
@@ -1676,7 +1683,7 @@
       <c r="C52" s="9">
         <v>41336</v>
       </c>
-      <c r="D52" s="12"/>
+      <c r="D52" s="27"/>
       <c r="E52" s="36"/>
       <c r="F52" s="11">
         <v>2</v>
@@ -1694,7 +1701,7 @@
       <c r="C53" s="9">
         <v>41336</v>
       </c>
-      <c r="D53" s="12"/>
+      <c r="D53" s="27"/>
       <c r="E53" s="36">
         <v>145</v>
       </c>
@@ -1715,7 +1722,7 @@
       <c r="C54" s="9">
         <v>41336</v>
       </c>
-      <c r="D54" s="12"/>
+      <c r="D54" s="27"/>
       <c r="E54" s="36"/>
       <c r="F54" s="11">
         <v>1</v>
@@ -1728,10 +1735,10 @@
       <c r="B55" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="27"/>
+      <c r="D55" s="26"/>
       <c r="E55" s="36"/>
       <c r="F55" s="11">
         <v>2</v>
@@ -1747,7 +1754,7 @@
       <c r="C56" s="9">
         <v>41336</v>
       </c>
-      <c r="D56" s="12"/>
+      <c r="D56" s="27"/>
       <c r="E56" s="36"/>
       <c r="F56" s="11">
         <v>3</v>
@@ -1763,7 +1770,7 @@
       <c r="C57" s="9">
         <v>41336</v>
       </c>
-      <c r="D57" s="12"/>
+      <c r="D57" s="26"/>
       <c r="E57" s="36"/>
       <c r="F57" s="11">
         <v>4</v>
@@ -1776,8 +1783,8 @@
       <c r="B58" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="12"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="27"/>
       <c r="E58" s="36"/>
       <c r="F58" s="11">
         <v>2</v>
@@ -1802,15 +1809,15 @@
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="33"/>
+      <c r="C60" s="39"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="25">
+      <c r="E60" s="24">
         <f>SUM(E12:E28)</f>
         <v>464</v>
       </c>
@@ -1819,15 +1826,15 @@
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="33"/>
+      <c r="C61" s="39"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="25">
+      <c r="E61" s="24">
         <f>SUM(E29:E46)</f>
         <v>442</v>
       </c>
@@ -1836,15 +1843,15 @@
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="33"/>
+      <c r="C62" s="39"/>
       <c r="D62" s="6"/>
-      <c r="E62" s="25">
+      <c r="E62" s="24">
         <f>SUM(E47:E58)</f>
         <v>285</v>
       </c>
@@ -1853,13 +1860,13 @@
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="C63" s="33"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
       <c r="D63" s="6"/>
-      <c r="E63" s="25">
+      <c r="E63" s="24">
         <f>SUM(E60:E62)</f>
         <v>1191</v>
       </c>
@@ -1874,75 +1881,75 @@
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
-      <c r="G64" s="26"/>
+      <c r="G64" s="25"/>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="32"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="32"/>
+      <c r="A69" s="35"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="35"/>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="32"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="35"/>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1957,45 +1964,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="G29:G34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="E35:E39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="E40:E46"/>
-    <mergeCell ref="G40:G46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="G47:G52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="E53:E59"/>
-    <mergeCell ref="G53:G59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
     <mergeCell ref="A68:A69"/>
     <mergeCell ref="C68:G68"/>
     <mergeCell ref="C69:G69"/>
@@ -2006,8 +1974,47 @@
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="B66:B67"/>
     <mergeCell ref="C66:G67"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="E53:E59"/>
+    <mergeCell ref="G53:G59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="E40:E46"/>
+    <mergeCell ref="G40:G46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="G47:G52"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="G29:G34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>